<commit_message>
working with dynamic paid
</commit_message>
<xml_diff>
--- a/Scheme_codes.xlsx
+++ b/Scheme_codes.xlsx
@@ -20,205 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
-  <si>
-    <t xml:space="preserve">AB1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB11 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB13 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB15 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB16 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AQ1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AQ2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN11 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN13 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BN9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ED1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG11 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG13 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG15 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FG9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FM2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FY1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FY2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FY2A </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS13 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS15 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS16 </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t xml:space="preserve">GS17 </t>
   </si>
@@ -704,8 +506,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,1023 +538,759 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+      <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+      <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+      <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+      <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+      <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+      <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+      <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+      <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+      <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+      <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+      <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+      <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
+      <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+      <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
+      <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
+      <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+      <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+      <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
+      <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>